<commit_message>
fix for right SP urls
</commit_message>
<xml_diff>
--- a/CapStatement/Argonaut_Capability_Statement_Clinical_Notes.xlsx
+++ b/CapStatement/Argonaut_Capability_Statement_Clinical_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06B4E9F-CABE-41EC-BE1B-6B5BDF25CE06}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1327FED1-11BB-4991-93AC-86D3FF9F6B58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="1860" windowWidth="23250" windowHeight="11055" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-25485" yWindow="585" windowWidth="23250" windowHeight="11055" activeTab="5" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -693,7 +693,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15F3286-55C1-40D0-93FC-C97EF26956B8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1066,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399C2ED-EDEB-47AB-8C1E-1290512B1D2F}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1410,7 @@
         <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
update Jinja 2 template, and spreadsheet to allow forbidden combos by resource
</commit_message>
<xml_diff>
--- a/CapStatement/Argonaut_Capability_Statement_Clinical_Notes.xlsx
+++ b/CapStatement/Argonaut_Capability_Statement_Clinical_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1327FED1-11BB-4991-93AC-86D3FF9F6B58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979D660-9140-4F33-BDFA-D1C1215ECE3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25485" yWindow="585" windowWidth="23250" windowHeight="11055" activeTab="5" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-28920" yWindow="-615" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="92">
   <si>
     <t>Value</t>
   </si>
@@ -276,9 +276,6 @@
   </si>
   <si>
     <t>ValueSet</t>
-  </si>
-  <si>
-    <t>patient,code,category</t>
   </si>
   <si>
     <t>combo_pairs</t>
@@ -293,12 +290,39 @@
 1. Declare a CapabilityStatement identifying the list of profiles, operations, search parameter supported.
 1. Support xml resource formats for all Argonaut questionnaire interactions.</t>
   </si>
+  <si>
+    <t>type,class,created</t>
+  </si>
+  <si>
+    <t>date,code,category</t>
+  </si>
+  <si>
+    <t>conf_Binary</t>
+  </si>
+  <si>
+    <t>patient,created</t>
+  </si>
+  <si>
+    <t>forbidden_s_combos</t>
+  </si>
+  <si>
+    <t>category,date|code,date</t>
+  </si>
+  <si>
+    <t>type,created|class,created</t>
+  </si>
+  <si>
+    <t>patient,category,code</t>
+  </si>
+  <si>
+    <t>The search parameters `created`, `class`, and `type`  MAY NOT be availabe as a *single* search parameter but SHALL be available in the combinations listed below.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +344,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="19"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -335,7 +365,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -358,12 +388,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF7E7E7E"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -375,6 +414,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -748,7 +790,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -769,10 +811,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B139EF60-0633-48C5-B394-C56F006BD6B3}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,6 +867,9 @@
         <v>69</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -833,10 +878,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB4CFA-AAEF-4FC6-A49B-107CEE80A317}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,9 +893,10 @@
     <col min="5" max="6" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -875,15 +921,20 @@
       <c r="H1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="D2" t="s">
         <v>36</v>
       </c>
@@ -893,8 +944,11 @@
       <c r="G2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -909,6 +963,26 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -926,7 +1000,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9E2E280-092F-4777-8984-8212A8DAB750}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C6:C7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,9 +1055,10 @@
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -991,10 +1066,13 @@
         <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1005,12 +1083,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1020,23 +1098,26 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1047,12 +1128,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1066,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7399C2ED-EDEB-47AB-8C1E-1290512B1D2F}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1134,7 +1215,7 @@
         <v>26</v>
       </c>
       <c r="Q1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1288,7 +1369,7 @@
         <v>31</v>
       </c>
       <c r="Q4" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1311,7 +1392,7 @@
         <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" ref="H5" si="1">A5&amp;"."&amp;C5</f>
@@ -1327,7 +1408,7 @@
         <v>31</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="M5" t="s">
         <v>31</v>
@@ -1395,6 +1476,9 @@
       <c r="P6" t="s">
         <v>31</v>
       </c>
+      <c r="Q6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1447,7 +1531,7 @@
         <v>31</v>
       </c>
       <c r="Q7" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1659,6 +1743,9 @@
       <c r="P11" t="s">
         <v>31</v>
       </c>
+      <c r="Q11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1711,7 +1798,7 @@
         <v>31</v>
       </c>
       <c r="Q12" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates jinj2  for clients
</commit_message>
<xml_diff>
--- a/CapStatement/Argonaut_Capability_Statement_Clinical_Notes.xlsx
+++ b/CapStatement/Argonaut_Capability_Statement_Clinical_Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10115"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eric\Documents\Python\MyNotebooks\CapStatement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/Python/MyNotebooks/CapStatement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2979D660-9140-4F33-BDFA-D1C1215ECE3D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A18504-C62B-A444-B0E7-E022B54239D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-615" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -315,7 +314,7 @@
     <t>patient,category,code</t>
   </si>
   <si>
-    <t>The search parameters `created`, `class`, and `type`  MAY NOT be availabe as a *single* search parameter but SHALL be available in the combinations listed below.</t>
+    <t>- The search parameters `created`, `class`, and `type`  MAY NOT be availabe as a *single* search parameter but SHALL be available in the combinations listed below.</t>
   </si>
 </sst>
 </file>
@@ -739,13 +738,13 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -753,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -761,7 +760,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -769,7 +768,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -777,7 +776,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -785,7 +784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="112" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -793,7 +792,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -817,15 +816,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="98.42578125" customWidth="1"/>
-    <col min="2" max="2" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="98.5" customWidth="1"/>
+    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -839,7 +838,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -853,7 +852,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>61</v>
       </c>
@@ -867,7 +866,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6"/>
     </row>
   </sheetData>
@@ -881,22 +880,22 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -925,7 +924,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -948,7 +947,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -969,7 +968,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1003,12 +1002,12 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1022,7 +1021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1050,15 +1049,15 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -1072,7 +1071,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1083,12 +1082,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1102,22 +1101,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1128,12 +1127,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -1151,21 +1150,21 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="63.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="34.7109375" customWidth="1"/>
-    <col min="9" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" customWidth="1"/>
-    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" customWidth="1"/>
+    <col min="8" max="8" width="34.6640625" customWidth="1"/>
+    <col min="9" max="15" width="9.1640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>72</v>
       </c>
@@ -1268,7 +1267,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1318,7 +1317,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1372,7 +1371,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -1426,7 +1425,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1480,7 +1479,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -1534,7 +1533,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1585,7 +1584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>69</v>
       </c>
@@ -1639,7 +1638,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>69</v>
       </c>
@@ -1693,7 +1692,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>69</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>69</v>
       </c>

</xml_diff>